<commit_message>
Bot level 2 Rocketbot full
</commit_message>
<xml_diff>
--- a/1. Documentos_ xml_xlsx/ProductosLibreria.xlsx
+++ b/1. Documentos_ xml_xlsx/ProductosLibreria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\users\yolima alejandra\desktop\robots\1. documentos_ xml_xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{954DA19B-DDE0-4C77-9DD2-593CDCBE1FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4A4720E1-9607-4AAD-9F08-403E126DFCF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
   <si>
     <t>Codigo</t>
   </si>
@@ -42,6 +42,9 @@
     <t>Costo_venta</t>
   </si>
   <si>
+    <t>Status</t>
+  </si>
+  <si>
     <t>P006</t>
   </si>
   <si>
@@ -49,9 +52,6 @@
   </si>
   <si>
     <t>Ciento</t>
-  </si>
-  <si>
-    <t>Status</t>
   </si>
   <si>
     <t>Ok</t>
@@ -391,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="A2" sqref="A2:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,18 +423,18 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>120000</v>
@@ -454,7 +454,7 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <v>80000</v>
@@ -463,6 +463,86 @@
         <v>100000</v>
       </c>
       <c r="F3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>120000</v>
+      </c>
+      <c r="E4">
+        <v>150000</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>80000</v>
+      </c>
+      <c r="E5">
+        <v>100000</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>120000</v>
+      </c>
+      <c r="E6">
+        <v>150000</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>80000</v>
+      </c>
+      <c r="E7">
+        <v>100000</v>
+      </c>
+      <c r="F7" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>